<commit_message>
generic retrieval pipeline update
</commit_message>
<xml_diff>
--- a/02_generic_data_compilation/results/generic_retrieval_results.xlsx
+++ b/02_generic_data_compilation/results/generic_retrieval_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,11 @@
           <t>Size (length or weight)</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Average annual surface temperature (tas)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -476,6 +481,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>10.36</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -485,7 +495,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Wetlands (inland) - Permanent Rivers/Streams/Creeks (includes waterfalls), Wetlands (inland) - Permanent Freshwater Marshes/Pools (under 8ha), Texas, Mexico, United States</t>
+          <t>Wetlands (inland) - Permanent Rivers/Streams/Creeks (includes waterfalls), Wetlands (inland) - Permanent Freshwater Marshes/Pools (under 8ha), Tamaulipas, Texas, Coahuila, Nuevo León, Mexico, United States</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -495,7 +505,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2.75 m</t>
+          <t>1.5 m</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>21.78</t>
         </is>
       </c>
     </row>
@@ -507,7 +522,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Marine Neritic - Seagrass (Submerged), Marine Neritic - Subtidal Loose Rock/pebble/gravel, Marine Neritic - Subtidal Rock and Rocky Reefs, Norway, Spain, Portugal, France, Germany, Italy, Greece, Türkiye, Syrian Arab Republic, Lebanon, Tunisia, Morocco, Malta, Jersey, Guernsey, Gibraltar, Denmark, Croatia, Bulgaria, Belgium, Albania, Monaco, Montenegro, Netherlands, Romania, Slovenia, Algeria, Egypt, Libya</t>
+          <t>Marine Neritic - Seagrass (Submerged), Marine Neritic - Subtidal Loose Rock/pebble/gravel, Marine Neritic - Subtidal Rock and Rocky Reefs, Norway, Portugal, Spain, Azores, Madeira, Canary Islands, France, Germany, Italy, Greece, Turkey, Bulgaria, Lebanon, Tunisia, Morocco, Malta, Jersey, Guernsey, Gibraltar, Denmark, Croatia, Belgium, Albania, Monaco, Montenegro, Netherlands, Romania, Slovenia, Algeria, Egypt, Libya</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -518,6 +533,11 @@
       <c r="D4" t="inlineStr">
         <is>
           <t>18 cm</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>15.01</t>
         </is>
       </c>
     </row>
@@ -539,7 +559,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>9.0 kg</t>
+          <t>7.375 kg</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>22.48</t>
         </is>
       </c>
     </row>
@@ -564,6 +589,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>12.23</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -586,6 +616,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -606,6 +641,11 @@
       <c r="D8" t="inlineStr">
         <is>
           <t>-</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>12.98</t>
         </is>
       </c>
     </row>

</xml_diff>